<commit_message>
Dodano skosnosc i kurtoze
</commit_message>
<xml_diff>
--- a/miary_obowiązkowe.xlsx
+++ b/miary_obowiązkowe.xlsx
@@ -177,13 +177,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -501,7 +498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -512,7 +509,7 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -524,100 +521,100 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="6"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="6"/>
+      <c r="A21" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>